<commit_message>
added 2019 to raw
</commit_message>
<xml_diff>
--- a/raw/colorado/accounting_reports.xlsx
+++ b/raw/colorado/accounting_reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20344"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\data\CA\usbr\lower colorado\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffh\OneDrive\Documents\UCDavis\data-surface-water\raw\colorado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713B0C8A-5B50-481D-B2B4-59EFC652A429}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4DCB32-1B0F-4322-BCBE-E5E48966C210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9300" windowHeight="2760" tabRatio="657" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" tabRatio="657" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entitlements" sheetId="6" r:id="rId1"/>
@@ -22,6 +22,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -190,11 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,14 +491,14 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="42.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="42.41796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.15625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -496,7 +506,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -504,7 +514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -513,7 +523,7 @@
         <v>11340</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -522,7 +532,7 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -530,7 +540,7 @@
         <v>262.8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -539,7 +549,7 @@
         <v>327000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -548,7 +558,7 @@
         <v>56846</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -557,7 +567,7 @@
         <v>16720</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -566,7 +576,7 @@
         <v>3288500</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -575,7 +585,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -584,7 +594,7 @@
         <v>1858.2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -593,7 +603,7 @@
         <v>634500</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -601,7 +611,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
@@ -609,7 +619,7 @@
         <v>112000</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -618,7 +628,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A18:A33">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:A33">
     <sortCondition ref="A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -628,623 +638,639 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AN17"/>
+  <dimension ref="A1:AO17"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="51.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8" style="2" customWidth="1"/>
-    <col min="5" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="18" width="9.140625" style="2"/>
-    <col min="19" max="19" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="51.15625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.15625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="8" style="2" customWidth="1"/>
+    <col min="6" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="19" width="9.15625" style="2"/>
+    <col min="20" max="20" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C1" s="1">
         <v>2018</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>2017</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>2016</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>2015</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>2014</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2013</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>2012</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>2011</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1">
         <v>2010</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
         <v>2009</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1">
         <v>2008</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N1" s="1">
         <v>2007</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="1">
         <v>2006</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>2005</v>
       </c>
-      <c r="P1" s="1">
+      <c r="Q1" s="1">
         <v>2004</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="R1" s="1">
         <v>2003</v>
       </c>
-      <c r="R1" s="1">
+      <c r="S1" s="1">
         <v>2002</v>
       </c>
-      <c r="S1" s="1">
+      <c r="T1" s="1">
         <v>2001</v>
       </c>
-      <c r="T1" s="1">
+      <c r="U1" s="1">
         <v>2000</v>
       </c>
-      <c r="U1" s="1">
+      <c r="V1" s="1">
         <v>1999</v>
       </c>
-      <c r="V1" s="1">
+      <c r="W1" s="1">
         <v>1998</v>
       </c>
-      <c r="W1" s="1">
+      <c r="X1" s="1">
         <v>1997</v>
       </c>
-      <c r="X1" s="1">
+      <c r="Y1" s="1">
         <v>1996</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Z1" s="1">
         <v>1995</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="AA1" s="1">
         <v>1994</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AB1" s="1">
         <v>1993</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AC1" s="1">
         <v>1992</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AD1" s="1">
         <v>1991</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AE1" s="1">
         <v>1990</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AF1" s="1">
         <v>1989</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AG1" s="1">
         <v>1988</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="AH1" s="1">
         <v>1987</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="AI1" s="1">
         <v>1986</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AJ1" s="1">
         <v>1985</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AK1" s="1">
         <v>1984</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AL1" s="1">
         <v>1983</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AM1" s="1">
         <v>1982</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AN1" s="1">
         <v>1981</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AO1" s="1">
         <v>1980</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
+        <v>9439</v>
+      </c>
+      <c r="C2" s="2">
         <v>14200</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>13781</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>11500</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>15115</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>16460</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>15259</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>15782</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>14762</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>11720</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>18099</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>14868</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>21275</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>18795</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>16282</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>16008</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>16435</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>16436</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>18457</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>23253</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>20959</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>26205</v>
       </c>
-      <c r="W2" s="2">
+      <c r="X2" s="2">
         <v>27241</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <v>30189</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Z2" s="2">
         <v>21364</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AA2" s="2">
         <v>22497</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AB2" s="2">
         <v>18725</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AC2" s="2">
         <v>20604</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AD2" s="2">
         <v>19704</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AE2" s="2">
         <v>20760</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AF2" s="2">
         <v>21072</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AG2" s="2">
         <v>22344</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AH2" s="2">
         <v>19578</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AI2" s="2">
         <v>20276</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AJ2" s="2">
         <v>16920</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="AK2" s="2">
         <v>20760</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="AL2" s="2">
         <v>22352</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="AM2" s="2">
         <v>20760</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AN2" s="2">
         <v>19128</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AO2" s="2">
         <v>11592</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
+        <v>1829</v>
+      </c>
+      <c r="C3" s="2">
         <v>1845</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>1887</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>1836</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>1819</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>2041</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>2200</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>2227</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>1975</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>2343</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>2441</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>2481</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>2587</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>2626</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>2461</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>2097</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>2583</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>2559</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>2717</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>2475</v>
       </c>
-      <c r="U3" s="2">
+      <c r="V3" s="2">
         <v>2588</v>
       </c>
-      <c r="V3" s="2">
+      <c r="W3" s="2">
         <v>2517</v>
       </c>
-      <c r="W3" s="2">
+      <c r="X3" s="2">
         <v>2833</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Y3" s="2">
         <v>3148</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Z3" s="2">
         <v>3119</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AA3" s="2">
         <v>3289</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AB3" s="2">
         <v>3709</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AC3" s="2">
         <f>2442+3373</f>
         <v>5815</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AD3" s="2">
         <v>3266</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AE3" s="2">
         <v>3267</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AF3" s="2">
         <v>3395</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AG3" s="2">
         <v>3203</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AH3" s="2">
         <v>2981</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="AI3" s="2">
         <v>2861</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AJ3" s="2">
         <v>3049</v>
       </c>
-      <c r="AJ3" s="2">
+      <c r="AK3" s="2">
         <v>3334</v>
       </c>
-      <c r="AK3" s="2">
+      <c r="AL3" s="2">
         <v>2917</v>
       </c>
-      <c r="AL3" s="2">
+      <c r="AM3" s="2">
         <v>3114</v>
       </c>
-      <c r="AM3" s="2">
+      <c r="AN3" s="2">
         <v>3092</v>
       </c>
-      <c r="AN3" s="2">
+      <c r="AO3" s="2">
         <v>2930</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
+        <v>153</v>
+      </c>
+      <c r="C4" s="2">
         <v>188</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>489</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>244</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>221</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>246</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>226</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>170</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>174</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>145</v>
-      </c>
-      <c r="K4" s="2">
-        <v>365</v>
       </c>
       <c r="L4" s="2">
         <v>365</v>
       </c>
       <c r="M4" s="2">
-        <v>294</v>
+        <v>365</v>
       </c>
       <c r="N4" s="2">
         <v>294</v>
       </c>
       <c r="O4" s="2">
+        <v>294</v>
+      </c>
+      <c r="P4" s="2">
         <v>1496</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>1444</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>621</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>89</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
         <v>216</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>342</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>265</v>
       </c>
-      <c r="V4" s="2">
+      <c r="W4" s="2">
         <v>664</v>
       </c>
-      <c r="W4" s="2">
+      <c r="X4" s="2">
         <v>252</v>
       </c>
-      <c r="X4" s="2">
+      <c r="Y4" s="2">
         <v>848</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
+        <v>540208</v>
+      </c>
+      <c r="C5" s="2">
         <v>891844</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>679767</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>999819</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>1181597</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>1179094</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>1015806</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>739017</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>542001</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>950083</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>967495</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <f>821212+6013</f>
         <v>827225</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <f>638664+4500</f>
         <v>643164</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <f>594544+172</f>
         <v>594716</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <f>839704+10000</f>
         <v>849704</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <f>733095+10000</f>
         <v>743095</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>688043</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>1241088</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
         <v>1253579</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>1303148</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <v>1215224</v>
       </c>
-      <c r="V5" s="2">
+      <c r="W5" s="2">
         <v>1076295</v>
       </c>
-      <c r="W5" s="2">
+      <c r="X5" s="2">
         <v>1241821</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Y5" s="2">
         <v>1230353</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Z5" s="2">
         <v>997414</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AA5" s="2">
         <v>1303212</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AB5" s="2">
         <v>1207331</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AC5" s="2">
         <v>1197422</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AD5" s="2">
         <v>1255720</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AE5" s="2">
         <v>1218321</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AF5" s="2">
         <v>1204578</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AG5" s="2">
         <v>1203571</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AH5" s="2">
         <v>1282277</v>
       </c>
-      <c r="AH5" s="2">
+      <c r="AI5" s="2">
         <v>1303276</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="AJ5" s="2">
         <v>1273236</v>
       </c>
-      <c r="AJ5" s="2">
+      <c r="AK5" s="2">
         <v>1237230</v>
       </c>
-      <c r="AK5" s="2">
+      <c r="AL5" s="2">
         <v>907564</v>
       </c>
-      <c r="AL5" s="2">
+      <c r="AM5" s="2">
         <v>716536</v>
       </c>
-      <c r="AM5" s="2">
+      <c r="AN5" s="2">
         <v>830228</v>
       </c>
-      <c r="AN5" s="2">
+      <c r="AO5" s="2">
         <v>821165</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>159965</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>151507</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>140188</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>80582</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>73125</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>40842</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>30000</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1261,1160 +1287,1191 @@
         <v>1</v>
       </c>
       <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
         <v>65</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>116</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>107</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>80</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <v>121</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <v>110</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>156</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>197</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>184</v>
-      </c>
-      <c r="O7" s="2">
-        <v>165</v>
       </c>
       <c r="P7" s="2">
         <v>165</v>
       </c>
       <c r="Q7" s="2">
+        <v>165</v>
+      </c>
+      <c r="R7" s="2">
         <v>156</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <v>165</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>167</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <v>205</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>141</v>
       </c>
-      <c r="V7" s="2">
+      <c r="W7" s="2">
         <v>121</v>
       </c>
-      <c r="W7" s="2">
+      <c r="X7" s="2">
         <v>189</v>
       </c>
-      <c r="X7" s="2">
+      <c r="Y7" s="2">
         <v>290</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Z7" s="2">
         <v>237</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AA7" s="2">
         <v>276</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AB7" s="2">
         <v>283</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AC7" s="2">
         <v>301</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AD7" s="2">
         <v>222</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AE7" s="2">
         <v>237</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="AF7" s="2">
         <v>308</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="AG7" s="2">
         <v>273</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="AH7" s="2">
         <v>255</v>
       </c>
-      <c r="AH7" s="2">
+      <c r="AI7" s="2">
         <v>238</v>
       </c>
-      <c r="AI7" s="2">
+      <c r="AJ7" s="2">
         <v>185</v>
       </c>
-      <c r="AJ7" s="2">
+      <c r="AK7" s="2">
         <v>171</v>
       </c>
-      <c r="AK7" s="2">
+      <c r="AL7" s="2">
         <v>143</v>
       </c>
-      <c r="AL7" s="2">
+      <c r="AM7" s="2">
         <v>228</v>
       </c>
-      <c r="AM7" s="2">
+      <c r="AN7" s="2">
         <v>280</v>
       </c>
-      <c r="AN7" s="2">
+      <c r="AO7" s="2">
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
+        <v>827</v>
+      </c>
+      <c r="C8" s="2">
         <v>1853</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="2">
         <v>2433</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="2">
         <v>4654</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>4522</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>4821</v>
-      </c>
-      <c r="G8" s="2">
-        <v>4740</v>
       </c>
       <c r="H8" s="2">
         <v>4740</v>
       </c>
       <c r="I8" s="2">
+        <v>4740</v>
+      </c>
+      <c r="J8" s="2">
         <v>4717</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>5693</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <f>4230+723</f>
         <v>4953</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <f>4230+753</f>
         <v>4983</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <f>4250+1346</f>
         <v>5596</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <f>4407+1426</f>
         <v>5833</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>5758</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="2">
         <f>4754+1477</f>
         <v>6231</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="R8" s="2">
         <f>2857+1551</f>
         <v>4408</v>
       </c>
-      <c r="R8" s="2">
+      <c r="S8" s="2">
         <f>2068+1652</f>
         <v>3720</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T8" s="2">
         <f>2643+1653</f>
         <v>4296</v>
       </c>
-      <c r="T8" s="2">
+      <c r="U8" s="2">
         <f>1839+1719</f>
         <v>3558</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <f>4117+1671</f>
         <v>5788</v>
       </c>
-      <c r="V8" s="2">
+      <c r="W8" s="2">
         <v>10937</v>
       </c>
-      <c r="W8" s="2">
+      <c r="X8" s="2">
         <v>4496</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Y8" s="2">
         <v>7320</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Z8" s="2">
         <v>8840</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AA8" s="2">
         <f>900+5801</f>
         <v>6701</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AB8" s="2">
         <v>7787</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AC8" s="2">
         <v>9793</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AD8" s="2">
         <f>906+7542</f>
         <v>8448</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AE8" s="2">
         <f>4156+1224</f>
         <v>5380</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AF8" s="2">
         <v>3682</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="AG8" s="2">
         <v>2450</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AH8" s="2">
         <f>4898+834</f>
         <v>5732</v>
       </c>
-      <c r="AH8" s="2">
+      <c r="AI8" s="2">
         <v>4035</v>
       </c>
-      <c r="AI8" s="2">
+      <c r="AJ8" s="2">
         <v>4923</v>
       </c>
-      <c r="AJ8" s="2">
+      <c r="AK8" s="2">
         <f>3670+890</f>
         <v>4560</v>
       </c>
-      <c r="AK8" s="2">
+      <c r="AL8" s="2">
         <f>3430+2224</f>
         <v>5654</v>
       </c>
-      <c r="AL8" s="2">
+      <c r="AM8" s="2">
         <v>3407</v>
       </c>
-      <c r="AM8" s="2">
+      <c r="AN8" s="2">
         <v>14046</v>
       </c>
-      <c r="AN8" s="2">
+      <c r="AO8" s="2">
         <f>10771+1270</f>
         <v>12041</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2">
+      <c r="B9" s="2">
+        <v>83</v>
+      </c>
+      <c r="D9" s="2">
         <v>97</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="2">
         <v>98</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>103</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>102</v>
-      </c>
-      <c r="I9" s="2">
-        <v>104</v>
       </c>
       <c r="J9" s="2">
         <v>104</v>
       </c>
       <c r="K9" s="2">
+        <v>104</v>
+      </c>
+      <c r="L9" s="2">
         <v>99</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>108</v>
-      </c>
-      <c r="M9" s="2">
-        <v>106</v>
       </c>
       <c r="N9" s="2">
         <v>106</v>
       </c>
       <c r="O9" s="2">
+        <v>106</v>
+      </c>
+      <c r="P9" s="2">
         <v>104</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>124</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>128</v>
       </c>
       <c r="R9" s="2">
         <v>128</v>
       </c>
       <c r="S9" s="2">
+        <v>128</v>
+      </c>
+      <c r="T9" s="2">
         <v>132</v>
-      </c>
-      <c r="T9" s="2">
-        <v>124</v>
       </c>
       <c r="U9" s="2">
         <v>124</v>
       </c>
       <c r="V9" s="2">
+        <v>124</v>
+      </c>
+      <c r="W9" s="2">
         <v>135</v>
       </c>
-      <c r="W9" s="2">
+      <c r="X9" s="2">
         <v>130</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Y9" s="2">
         <v>136</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Z9" s="2">
         <v>129</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AA9" s="2">
         <v>134</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AB9" s="2">
         <v>120</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AC9" s="2">
         <v>126</v>
       </c>
-      <c r="AC9" s="2">
+      <c r="AD9" s="2">
         <v>129</v>
       </c>
-      <c r="AD9" s="2">
+      <c r="AE9" s="2">
         <v>125</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="AF9" s="2">
         <v>142</v>
       </c>
-      <c r="AF9" s="2">
+      <c r="AG9" s="2">
         <v>127</v>
       </c>
-      <c r="AG9" s="2">
+      <c r="AH9" s="2">
         <v>122</v>
-      </c>
-      <c r="AH9" s="2">
-        <v>101</v>
       </c>
       <c r="AI9" s="2">
         <v>101</v>
       </c>
       <c r="AJ9" s="2">
+        <v>101</v>
+      </c>
+      <c r="AK9" s="2">
         <v>80</v>
       </c>
-      <c r="AK9" s="2">
+      <c r="AL9" s="2">
         <v>113</v>
       </c>
-      <c r="AL9" s="2">
+      <c r="AM9" s="2">
         <v>119</v>
       </c>
-      <c r="AM9" s="2">
+      <c r="AN9" s="2">
         <v>140</v>
       </c>
-      <c r="AN9" s="2">
+      <c r="AO9" s="2">
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="4">
+        <v>799070</v>
+      </c>
+      <c r="C10" s="2">
         <v>771370</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>732870</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="2">
         <v>775220</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>866840</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>948630</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>972270</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>893880</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>810260</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>716600</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>746790</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>881220</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>917090</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>851320</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <v>800460</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>969040</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
         <v>917360</v>
       </c>
-      <c r="R10" s="2">
+      <c r="S10" s="2">
         <v>998610</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T10" s="2">
         <v>944740</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <v>962760</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <v>938870</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <v>918910</v>
       </c>
-      <c r="W10" s="2">
+      <c r="X10" s="2">
         <v>917520</v>
       </c>
-      <c r="X10" s="2">
+      <c r="Y10" s="2">
         <v>953010</v>
       </c>
-      <c r="Y10" s="2">
+      <c r="Z10" s="2">
         <v>861800</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="AA10" s="2">
         <v>800370</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AB10" s="2">
         <v>737100</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AC10" s="2">
         <v>768160</v>
       </c>
-      <c r="AC10" s="2">
+      <c r="AD10" s="2">
         <v>851920</v>
       </c>
-      <c r="AD10" s="2">
+      <c r="AE10" s="2">
         <v>917480</v>
       </c>
-      <c r="AE10" s="2">
+      <c r="AF10" s="2">
         <v>935426</v>
       </c>
-      <c r="AF10" s="2">
+      <c r="AG10" s="2">
         <v>898650</v>
       </c>
-      <c r="AG10" s="2">
+      <c r="AH10" s="2">
         <v>864570</v>
       </c>
-      <c r="AH10" s="2">
+      <c r="AI10" s="2">
         <v>872976</v>
       </c>
-      <c r="AI10" s="2">
+      <c r="AJ10" s="2">
         <v>879896</v>
       </c>
-      <c r="AJ10" s="2">
+      <c r="AK10" s="2">
         <v>834905</v>
       </c>
-      <c r="AK10" s="2">
+      <c r="AL10" s="2">
         <v>786664</v>
       </c>
-      <c r="AL10" s="2">
+      <c r="AM10" s="2">
         <v>941974</v>
       </c>
-      <c r="AM10" s="2">
+      <c r="AN10" s="2">
         <v>1007553</v>
       </c>
-      <c r="AN10" s="2">
+      <c r="AO10" s="2">
         <v>906455</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AB11" s="2">
+      <c r="AC11" s="2">
         <v>113</v>
       </c>
-      <c r="AC11" s="2">
+      <c r="AD11" s="2">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2">
+        <v>44018</v>
+      </c>
+      <c r="C12" s="2">
         <v>42639</v>
       </c>
-      <c r="C12" s="2">
+      <c r="D12" s="2">
         <v>44440</v>
       </c>
-      <c r="D12" s="2">
+      <c r="E12" s="2">
         <v>44781</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>47047</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>47195</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>46367</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>45443</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>44247</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <f>40761+795</f>
         <v>41556</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <f>37023+795</f>
         <v>37818</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <f>45249+795</f>
         <v>46044</v>
       </c>
-      <c r="M12" s="2">
+      <c r="N12" s="2">
         <f>44496+794</f>
         <v>45290</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>38187</v>
       </c>
-      <c r="O12" s="2">
+      <c r="P12" s="2">
         <v>44803</v>
       </c>
-      <c r="P12" s="2">
+      <c r="Q12" s="2">
         <v>46256</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="R12" s="2">
         <v>46352</v>
       </c>
-      <c r="R12" s="2">
+      <c r="S12" s="2">
         <v>47084</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T12" s="2">
         <v>40992</v>
       </c>
-      <c r="T12" s="2">
+      <c r="U12" s="2">
         <v>31269</v>
       </c>
-      <c r="U12" s="2">
+      <c r="V12" s="2">
         <v>31350</v>
       </c>
-      <c r="V12" s="2">
+      <c r="W12" s="2">
         <v>31386</v>
       </c>
-      <c r="W12" s="2">
+      <c r="X12" s="2">
         <v>31008</v>
       </c>
-      <c r="X12" s="2">
+      <c r="Y12" s="2">
         <v>33196</v>
       </c>
-      <c r="Y12" s="2">
+      <c r="Z12" s="2">
         <v>38939</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="AA12" s="2">
         <v>49374</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AB12" s="2">
         <v>45475</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AC12" s="2">
         <v>49572</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="AD12" s="2">
         <v>49613</v>
       </c>
-      <c r="AD12" s="2">
+      <c r="AE12" s="2">
         <v>49638</v>
       </c>
-      <c r="AE12" s="2">
+      <c r="AF12" s="2">
         <v>63558</v>
       </c>
-      <c r="AF12" s="2">
+      <c r="AG12" s="2">
         <v>43888</v>
       </c>
-      <c r="AG12" s="2">
+      <c r="AH12" s="2">
         <v>32381</v>
-      </c>
-      <c r="AH12" s="2">
-        <v>29896</v>
       </c>
       <c r="AI12" s="2">
         <v>29896</v>
       </c>
       <c r="AJ12" s="2">
+        <v>29896</v>
+      </c>
+      <c r="AK12" s="2">
         <v>26751</v>
       </c>
-      <c r="AK12" s="2">
+      <c r="AL12" s="2">
         <v>22485</v>
       </c>
-      <c r="AL12" s="2">
+      <c r="AM12" s="2">
         <v>40005</v>
       </c>
-      <c r="AM12" s="2">
+      <c r="AN12" s="2">
         <v>43767</v>
       </c>
-      <c r="AN12" s="2">
+      <c r="AO12" s="2">
         <v>42432</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2">
+        <v>36261</v>
+      </c>
+      <c r="C13" s="2">
         <v>42952</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>37986</v>
       </c>
-      <c r="D13" s="2">
+      <c r="E13" s="2">
         <v>47709</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>48561</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>51080</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>49512</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>50729</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>49552</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>39551</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>43550</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>44568</v>
       </c>
-      <c r="M13" s="2">
+      <c r="N13" s="2">
         <v>43454</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>40757</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>38537</v>
       </c>
-      <c r="P13" s="2">
+      <c r="Q13" s="2">
         <v>37457</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="R13" s="2">
         <v>46977</v>
       </c>
-      <c r="R13" s="2">
+      <c r="S13" s="2">
         <v>47221</v>
       </c>
-      <c r="S13" s="2">
+      <c r="T13" s="2">
         <v>46180</v>
       </c>
-      <c r="T13" s="2">
+      <c r="U13" s="2">
         <v>50863</v>
       </c>
-      <c r="U13" s="2">
+      <c r="V13" s="2">
         <v>48800</v>
       </c>
-      <c r="V13" s="2">
+      <c r="W13" s="2">
         <v>49812</v>
       </c>
-      <c r="W13" s="2">
+      <c r="X13" s="2">
         <v>53179</v>
       </c>
-      <c r="X13" s="2">
+      <c r="Y13" s="2">
         <v>56412</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Z13" s="2">
         <v>52843</v>
       </c>
-      <c r="Z13" s="2">
+      <c r="AA13" s="2">
         <v>55610</v>
       </c>
-      <c r="AA13" s="2">
+      <c r="AB13" s="2">
         <v>51510</v>
       </c>
-      <c r="AB13" s="2">
+      <c r="AC13" s="2">
         <v>46442</v>
       </c>
-      <c r="AC13" s="2">
+      <c r="AD13" s="2">
         <v>53966</v>
       </c>
-      <c r="AD13" s="2">
+      <c r="AE13" s="2">
         <v>52886</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="AF13" s="2">
         <v>40017</v>
       </c>
-      <c r="AF13" s="2">
+      <c r="AG13" s="2">
         <v>53226</v>
       </c>
-      <c r="AG13" s="2">
+      <c r="AH13" s="2">
         <v>49048</v>
-      </c>
-      <c r="AH13" s="2">
-        <v>46293</v>
       </c>
       <c r="AI13" s="2">
         <v>46293</v>
       </c>
       <c r="AJ13" s="2">
+        <v>46293</v>
+      </c>
+      <c r="AK13" s="2">
         <v>40452</v>
       </c>
-      <c r="AK13" s="2">
+      <c r="AL13" s="2">
         <v>40667</v>
       </c>
-      <c r="AL13" s="2">
+      <c r="AM13" s="2">
         <v>47811</v>
       </c>
-      <c r="AM13" s="2">
+      <c r="AN13" s="2">
         <v>50740</v>
       </c>
-      <c r="AN13" s="2">
+      <c r="AO13" s="2">
         <v>47676</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="4">
+        <v>2529797</v>
+      </c>
+      <c r="C14" s="2">
         <v>2515215</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D14" s="2">
         <v>2488615</v>
       </c>
-      <c r="D14" s="2">
+      <c r="E14" s="2">
         <v>2461562</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>2455649</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>2496428</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>2535452</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>2897602</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>2899353</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>2640769</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>2679356</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>2919108</v>
       </c>
-      <c r="M14" s="2">
+      <c r="N14" s="2">
         <v>2952526</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>2994325</v>
       </c>
-      <c r="O14" s="2">
+      <c r="P14" s="2">
         <v>2860526</v>
       </c>
-      <c r="P14" s="2">
+      <c r="Q14" s="2">
         <v>2822794</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="R14" s="2">
         <v>3066361</v>
       </c>
-      <c r="R14" s="2">
+      <c r="S14" s="2">
         <v>3230352</v>
       </c>
-      <c r="S14" s="2">
+      <c r="T14" s="2">
         <v>3190927</v>
       </c>
-      <c r="T14" s="2">
+      <c r="U14" s="2">
         <v>3162184</v>
       </c>
-      <c r="U14" s="2">
+      <c r="V14" s="2">
         <v>3122480</v>
       </c>
-      <c r="V14" s="2">
+      <c r="W14" s="2">
         <v>3148164</v>
       </c>
-      <c r="W14" s="2">
+      <c r="X14" s="2">
         <v>3235259</v>
       </c>
-      <c r="X14" s="2">
+      <c r="Y14" s="2">
         <v>3275453</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Z14" s="2">
         <v>3171927</v>
       </c>
-      <c r="Z14" s="2">
+      <c r="AA14" s="2">
         <v>3172082</v>
       </c>
-      <c r="AA14" s="2">
+      <c r="AB14" s="2">
         <v>2886565</v>
       </c>
-      <c r="AB14" s="2">
+      <c r="AC14" s="2">
         <v>2675901</v>
       </c>
-      <c r="AC14" s="2">
+      <c r="AD14" s="2">
         <v>2985723</v>
       </c>
-      <c r="AD14" s="2">
+      <c r="AE14" s="2">
         <v>3135301</v>
       </c>
-      <c r="AE14" s="2">
+      <c r="AF14" s="2">
         <v>3085811</v>
       </c>
-      <c r="AF14" s="2">
+      <c r="AG14" s="2">
         <v>3014187</v>
       </c>
-      <c r="AG14" s="2">
+      <c r="AH14" s="2">
         <v>2815986</v>
-      </c>
-      <c r="AH14" s="2">
-        <v>2717913</v>
       </c>
       <c r="AI14" s="2">
         <v>2717913</v>
       </c>
       <c r="AJ14" s="2">
+        <v>2717913</v>
+      </c>
+      <c r="AK14" s="2">
         <v>2682700</v>
       </c>
-      <c r="AK14" s="2">
+      <c r="AL14" s="2">
         <v>2555617</v>
       </c>
-      <c r="AL14" s="2">
+      <c r="AM14" s="2">
         <v>2595578</v>
       </c>
-      <c r="AM14" s="2">
+      <c r="AN14" s="2">
         <v>2872289</v>
       </c>
-      <c r="AN14" s="2">
+      <c r="AO14" s="2">
         <v>2845779</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2">
         <v>150</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>110424</v>
       </c>
-      <c r="D15" s="2">
+      <c r="E15" s="2">
         <v>135819</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>163810</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>94037</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>75015</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>16081</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>0</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>83462</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>31700</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>27173</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <v>23871</v>
-      </c>
-      <c r="N15" s="2">
-        <v>0</v>
       </c>
       <c r="O15" s="2">
         <v>0</v>
       </c>
       <c r="P15" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="2">
         <v>14929</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
+        <v>358675</v>
+      </c>
+      <c r="C16" s="2">
         <v>346367</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>343930</v>
       </c>
-      <c r="D16" s="2">
+      <c r="E16" s="2">
         <v>372371</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>360381</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>366779</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>345604</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>344923</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>320573</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>319098</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>322730</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>310159</v>
       </c>
-      <c r="M16" s="2">
+      <c r="N16" s="2">
         <v>321174</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <v>339065</v>
       </c>
-      <c r="O16" s="2">
+      <c r="P16" s="2">
         <v>316479</v>
       </c>
-      <c r="P16" s="2">
+      <c r="Q16" s="2">
         <v>328333</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="R16" s="2">
         <v>305923</v>
       </c>
-      <c r="R16" s="2">
+      <c r="S16" s="2">
         <v>339506</v>
       </c>
-      <c r="S16" s="2">
+      <c r="T16" s="2">
         <v>335932</v>
       </c>
-      <c r="T16" s="2">
+      <c r="U16" s="2">
         <v>348747</v>
       </c>
-      <c r="U16" s="2">
+      <c r="V16" s="2">
         <v>337509</v>
       </c>
-      <c r="V16" s="2">
+      <c r="W16" s="2">
         <v>342597</v>
       </c>
-      <c r="W16" s="2">
+      <c r="X16" s="2">
         <v>346489</v>
       </c>
-      <c r="X16" s="2">
+      <c r="Y16" s="2">
         <v>343828</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Z16" s="2">
         <v>337805</v>
       </c>
-      <c r="Z16" s="2">
+      <c r="AA16" s="2">
         <v>339530</v>
       </c>
-      <c r="AA16" s="2">
+      <c r="AB16" s="2">
         <v>332654</v>
       </c>
-      <c r="AB16" s="2">
+      <c r="AC16" s="2">
         <v>321955</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="AD16" s="2">
         <v>327417</v>
       </c>
-      <c r="AD16" s="2">
+      <c r="AE16" s="2">
         <v>379619</v>
       </c>
-      <c r="AE16" s="2">
+      <c r="AF16" s="2">
         <v>368590</v>
       </c>
-      <c r="AF16" s="2">
+      <c r="AG16" s="2">
         <v>339311</v>
       </c>
-      <c r="AG16" s="2">
+      <c r="AH16" s="2">
         <v>338754</v>
-      </c>
-      <c r="AH16" s="2">
-        <v>341040</v>
       </c>
       <c r="AI16" s="2">
         <v>341040</v>
       </c>
       <c r="AJ16" s="2">
+        <v>341040</v>
+      </c>
+      <c r="AK16" s="2">
         <v>357975</v>
       </c>
-      <c r="AK16" s="2">
+      <c r="AL16" s="2">
         <v>362266</v>
       </c>
-      <c r="AL16" s="2">
+      <c r="AM16" s="2">
         <v>424868</v>
       </c>
-      <c r="AM16" s="2">
+      <c r="AN16" s="2">
         <v>452260</v>
       </c>
-      <c r="AN16" s="2">
+      <c r="AO16" s="2">
         <v>531791</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="2">
-        <f>4639003-SUM(B2:B16)</f>
+        <f>4329425-SUM(B2:B16)</f>
+        <v>9047</v>
+      </c>
+      <c r="C17" s="2">
+        <f>4639003-SUM(C2:C16)</f>
         <v>10379</v>
       </c>
-      <c r="C17" s="2">
-        <f>4467987-SUM(C2:C16)</f>
+      <c r="D17" s="2">
+        <f>4467987-SUM(D2:D16)</f>
         <v>11267</v>
       </c>
-      <c r="D17" s="2">
-        <f>4868599-SUM(D2:D16)</f>
+      <c r="E17" s="2">
+        <f>4868599-SUM(E2:E16)</f>
         <v>12985</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>11437</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>13256</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>13707</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>14718</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>12065</v>
       </c>
-      <c r="J17" s="2">
+      <c r="K17" s="2">
         <v>8425</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>16492</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>18203</v>
       </c>
-      <c r="M17" s="2">
+      <c r="N17" s="2">
         <v>18993</v>
       </c>
-      <c r="N17" s="2">
+      <c r="O17" s="2">
         <v>18963</v>
       </c>
-      <c r="O17" s="2">
+      <c r="P17" s="2">
         <v>21360</v>
       </c>
-      <c r="P17" s="2">
+      <c r="Q17" s="2">
         <v>22436</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="R17" s="2">
         <v>21208</v>
       </c>
-      <c r="R17" s="2">
+      <c r="S17" s="2">
         <v>20000</v>
       </c>
-      <c r="S17" s="2">
+      <c r="T17" s="2">
         <v>17850</v>
       </c>
-      <c r="T17" s="2">
+      <c r="U17" s="2">
         <v>20561</v>
       </c>
-      <c r="U17" s="2">
+      <c r="V17" s="2">
         <v>19590</v>
       </c>
-      <c r="V17" s="2">
+      <c r="W17" s="2">
         <v>21687</v>
       </c>
-      <c r="W17" s="2">
+      <c r="X17" s="2">
         <v>17799</v>
       </c>
-      <c r="X17" s="2">
+      <c r="Y17" s="2">
         <v>23950</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="Z17" s="2">
         <v>25081</v>
       </c>
-      <c r="Z17" s="2">
+      <c r="AA17" s="2">
         <v>25261</v>
       </c>
-      <c r="AA17" s="2">
+      <c r="AB17" s="2">
         <v>26381</v>
       </c>
-      <c r="AB17" s="2">
+      <c r="AC17" s="2">
         <v>21603</v>
       </c>
-      <c r="AC17" s="2">
+      <c r="AD17" s="2">
         <v>30014</v>
       </c>
-      <c r="AD17" s="2">
+      <c r="AE17" s="2">
         <v>23518</v>
       </c>
-      <c r="AE17" s="2">
+      <c r="AF17" s="2">
         <v>21994</v>
       </c>
-      <c r="AF17" s="2">
+      <c r="AG17" s="2">
         <v>19139</v>
       </c>
-      <c r="AG17" s="2">
+      <c r="AH17" s="2">
         <v>18933</v>
       </c>
-      <c r="AH17" s="2">
+      <c r="AI17" s="2">
         <v>15864</v>
       </c>
-      <c r="AI17" s="2">
+      <c r="AJ17" s="2">
         <v>17473</v>
       </c>
-      <c r="AJ17" s="2">
+      <c r="AK17" s="2">
         <v>14341</v>
       </c>
-      <c r="AK17" s="2">
+      <c r="AL17" s="2">
         <v>16644</v>
       </c>
-      <c r="AL17" s="2">
+      <c r="AM17" s="2">
         <v>20661</v>
       </c>
-      <c r="AM17" s="2">
+      <c r="AN17" s="2">
         <v>23924</v>
       </c>
-      <c r="AN17" s="2">
+      <c r="AO17" s="2">
         <v>24447</v>
       </c>
     </row>
@@ -2426,760 +2483,779 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AN6"/>
+  <dimension ref="A1:AO6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="51.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8" style="2" customWidth="1"/>
-    <col min="5" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="51.15625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.15625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8" style="2" customWidth="1"/>
+    <col min="6" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C1" s="1">
         <v>2018</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="1">
         <v>2017</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="1">
         <v>2016</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>2015</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>2014</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2013</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>2012</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>2011</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1">
         <v>2010</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
         <v>2009</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1">
         <v>2008</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N1" s="1">
         <v>2007</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="1">
         <v>2006</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>2005</v>
       </c>
-      <c r="P1" s="1">
+      <c r="Q1" s="1">
         <v>2004</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="R1" s="1">
         <v>2003</v>
       </c>
-      <c r="R1" s="1">
+      <c r="S1" s="1">
         <v>2002</v>
       </c>
-      <c r="S1" s="1">
+      <c r="T1" s="1">
         <v>2001</v>
       </c>
-      <c r="T1" s="1">
+      <c r="U1" s="1">
         <v>2000</v>
       </c>
-      <c r="U1" s="1">
+      <c r="V1" s="1">
         <v>1999</v>
       </c>
-      <c r="V1" s="1">
+      <c r="W1" s="1">
         <v>1998</v>
       </c>
-      <c r="W1" s="1">
+      <c r="X1" s="1">
         <v>1997</v>
       </c>
-      <c r="X1" s="1">
+      <c r="Y1" s="1">
         <v>1996</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Z1" s="1">
         <v>1995</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="AA1" s="1">
         <v>1994</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AB1" s="1">
         <v>1993</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AC1" s="1">
         <v>1992</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AD1" s="1">
         <v>1991</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AE1" s="1">
         <v>1990</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AF1" s="1">
         <v>1989</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AG1" s="1">
         <v>1988</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="AH1" s="1">
         <v>1987</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="AI1" s="1">
         <v>1986</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AJ1" s="1">
         <v>1985</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AK1" s="1">
         <v>1984</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AL1" s="1">
         <v>1983</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AM1" s="1">
         <v>1982</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AN1" s="1">
         <v>1981</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AO1" s="1">
         <v>1980</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
+        <v>25825</v>
+      </c>
+      <c r="C2" s="2">
         <v>67086</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>16188</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>43297</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>31765</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>18214</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>4151</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>8981</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>25583</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>27957</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>68311</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>43486</v>
       </c>
-      <c r="M2" s="2">
+      <c r="N2" s="2">
         <v>39617</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>16852</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>45218</v>
       </c>
-      <c r="P2" s="2">
+      <c r="Q2" s="2">
         <v>36421</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>2911</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>20600</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>45100</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>5800</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>36600</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>39500</v>
       </c>
-      <c r="W2" s="2">
+      <c r="X2" s="2">
         <v>4667</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <v>46119</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Z2" s="2">
         <v>48051</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AA2" s="2">
         <v>25370</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AB2" s="2">
         <v>33750</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AC2" s="2">
         <v>4882</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AD2" s="2">
         <v>4746</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AE2" s="2">
         <v>25518</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AF2" s="2">
         <v>2618</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AG2" s="2">
         <v>16090</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="AH2" s="2">
         <v>48233</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AI2" s="2">
         <v>60154</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AJ2" s="2">
         <v>33022</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="AK2" s="2">
         <v>48570</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="AL2" s="2">
         <v>53652</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="AM2" s="2">
         <v>13228</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="AN2" s="2">
         <v>9582</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="AO2" s="2">
         <v>11082</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
+        <v>20297</v>
+      </c>
+      <c r="C3" s="2">
         <v>11773</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>9371</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>13709</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>11527</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>8937</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>7289</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>6763</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>9333</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>7773</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>12073</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>11910</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>10433</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>33072</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>40023</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>19366</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>35532</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>24598</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>34708</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>19200</v>
       </c>
-      <c r="U3" s="2">
+      <c r="V3" s="2">
         <v>36444</v>
       </c>
-      <c r="V3" s="2">
+      <c r="W3" s="2">
         <v>35467</v>
       </c>
-      <c r="W3" s="2">
+      <c r="X3" s="2">
         <v>33094</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Y3" s="2">
         <v>17696</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Z3" s="2">
         <v>33424</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AA3" s="2">
         <v>25636</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AB3" s="2">
         <v>23063</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AC3" s="2">
         <v>11512</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AD3" s="2">
         <v>22775</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AE3" s="2">
         <v>18517</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AF3" s="2">
         <v>29167</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AG3" s="2">
         <v>41925</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AH3" s="2">
         <v>38104</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="AI3" s="2">
         <v>43975</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AJ3" s="2">
         <v>40844</v>
       </c>
-      <c r="AJ3" s="2">
+      <c r="AK3" s="2">
         <v>54400</v>
       </c>
-      <c r="AK3" s="2">
+      <c r="AL3" s="2">
         <v>40250</v>
       </c>
-      <c r="AL3" s="2">
+      <c r="AM3" s="2">
         <v>18344</v>
       </c>
-      <c r="AM3" s="2">
+      <c r="AN3" s="2">
         <v>8370</v>
       </c>
-      <c r="AN3" s="2">
+      <c r="AO3" s="2">
         <v>8800</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
+        <v>31443</v>
+      </c>
+      <c r="C4" s="2">
         <v>27134</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>38584</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>39113</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>36233</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>25709</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>26648</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>31631</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>28265</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>32183</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>30091</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>38444</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>34247</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>38139</v>
       </c>
-      <c r="O4" s="2">
+      <c r="P4" s="2">
         <v>37110</v>
       </c>
-      <c r="P4" s="2">
+      <c r="Q4" s="2">
         <v>36845</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>46593</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>23678</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
         <v>21939</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>24121</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>28574</v>
       </c>
-      <c r="V4" s="2">
+      <c r="W4" s="2">
         <v>25868</v>
       </c>
-      <c r="W4" s="2">
+      <c r="X4" s="2">
         <v>27401</v>
       </c>
-      <c r="X4" s="2">
+      <c r="Y4" s="2">
         <v>20527</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Z4" s="2">
         <v>26775</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AA4" s="2">
         <v>27419</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AB4" s="2">
         <v>21833</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AC4" s="2">
         <v>27363</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AD4" s="2">
         <v>23317</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AE4" s="2">
         <v>19493</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AF4" s="2">
         <v>16162</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AG4" s="2">
         <v>24011</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="AH4" s="2">
         <f>14844+9626</f>
         <v>24470</v>
       </c>
-      <c r="AH4" s="2">
+      <c r="AI4" s="2">
         <f>13632+8129</f>
         <v>21761</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="AJ4" s="2">
         <f>12509+7941</f>
         <v>20450</v>
       </c>
-      <c r="AJ4" s="2">
+      <c r="AK4" s="2">
         <f>13961+9431</f>
         <v>23392</v>
       </c>
-      <c r="AK4" s="2">
+      <c r="AL4" s="2">
         <f>14082+7808</f>
         <v>21890</v>
       </c>
-      <c r="AL4" s="2">
+      <c r="AM4" s="2">
         <f>12201+9375</f>
         <v>21576</v>
       </c>
-      <c r="AM4" s="2">
+      <c r="AN4" s="2">
         <f>11958+9806</f>
         <v>21764</v>
       </c>
-      <c r="AN4" s="2">
+      <c r="AO4" s="2">
         <f>7564+6285</f>
         <v>13849</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="4">
+        <v>263681</v>
+      </c>
+      <c r="C5" s="2">
         <v>315256</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>236673</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>302948</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>283611</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>333754</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>286674</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>190873</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>184660</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>304723</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>192668</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>154537</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>105705</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>116993</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>112347</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>159830</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>109103</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>100995</v>
       </c>
-      <c r="S5" s="2">
+      <c r="T5" s="2">
         <v>97894</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>92592</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <v>89871</v>
       </c>
-      <c r="V5" s="2">
+      <c r="W5" s="2">
         <v>84117</v>
       </c>
-      <c r="W5" s="2">
+      <c r="X5" s="2">
         <v>70434</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Y5" s="2">
         <v>31745</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Z5" s="2">
         <v>45222</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AA5" s="2">
         <v>74513</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AB5" s="2">
         <v>51341</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AC5" s="2">
         <v>97015</v>
       </c>
-      <c r="AC5" s="2">
+      <c r="AD5" s="2">
         <v>70344</v>
       </c>
-      <c r="AD5" s="2">
+      <c r="AE5" s="2">
         <v>34381</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AF5" s="2">
         <v>38040</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="AG5" s="2">
         <v>44795</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="AH5" s="2">
         <v>47596</v>
       </c>
-      <c r="AH5" s="2">
+      <c r="AI5" s="2">
         <v>69482</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="AJ5" s="2">
         <v>59413</v>
       </c>
-      <c r="AJ5" s="2">
+      <c r="AK5" s="2">
         <v>46293</v>
       </c>
-      <c r="AK5" s="2">
+      <c r="AL5" s="2">
         <v>132561</v>
       </c>
-      <c r="AL5" s="2">
+      <c r="AM5" s="2">
         <v>57712</v>
       </c>
-      <c r="AM5" s="2">
+      <c r="AN5" s="2">
         <v>48942</v>
       </c>
-      <c r="AN5" s="2">
+      <c r="AO5" s="2">
         <v>67429</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:41" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="4">
+        <v>16109</v>
+      </c>
+      <c r="C6" s="2">
         <v>28654</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>22587</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>23353</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>34743</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>43123</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>21410</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>32360</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>43168</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>72246</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>29010</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>38234</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>23842</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>16567</v>
       </c>
-      <c r="O6" s="2">
+      <c r="P6" s="2">
         <v>8202</v>
       </c>
-      <c r="P6" s="2">
+      <c r="Q6" s="2">
         <v>15206</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>8480</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <v>8066</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>8675</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>9635</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <v>11753</v>
       </c>
-      <c r="V6" s="2">
+      <c r="W6" s="2">
         <v>4855</v>
       </c>
-      <c r="W6" s="2">
+      <c r="X6" s="2">
         <v>9535</v>
       </c>
-      <c r="X6" s="2">
+      <c r="Y6" s="2">
         <v>5497</v>
       </c>
-      <c r="Y6" s="2">
+      <c r="Z6" s="2">
         <v>4449</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AA6" s="2">
         <v>5613</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AB6" s="2">
         <v>5652</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AC6" s="2">
         <v>6771</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AD6" s="2">
         <v>8148</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AE6" s="2">
         <v>5162</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="AF6" s="2">
         <v>6165</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="AG6" s="2">
         <v>12059</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="AH6" s="2">
         <v>9607</v>
       </c>
-      <c r="AH6" s="2">
+      <c r="AI6" s="2">
         <v>10359</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="AJ6" s="2">
         <v>9684</v>
       </c>
-      <c r="AJ6" s="2">
+      <c r="AK6" s="2">
         <v>19337</v>
       </c>
-      <c r="AK6" s="2">
+      <c r="AL6" s="2">
         <v>23344</v>
       </c>
-      <c r="AL6" s="2">
+      <c r="AM6" s="2">
         <v>7457</v>
       </c>
-      <c r="AM6" s="2">
+      <c r="AN6" s="2">
         <v>11590</v>
       </c>
-      <c r="AN6" s="2">
+      <c r="AO6" s="2">
         <v>15353</v>
       </c>
     </row>
@@ -3191,25 +3267,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AP15"/>
+  <dimension ref="A1:AQ15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8" style="2" customWidth="1"/>
-    <col min="7" max="8" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="50.3671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.89453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.89453125" style="2" customWidth="1"/>
+    <col min="5" max="7" width="8" style="2" customWidth="1"/>
+    <col min="8" max="9" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.15625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -3220,124 +3298,127 @@
         <v>22</v>
       </c>
       <c r="D1" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E1" s="1">
         <v>2018</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="1">
         <v>2017</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
         <v>2016</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="1">
         <v>2015</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="1">
         <v>2014</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="1">
         <v>2013</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="1">
         <v>2012</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L1" s="1">
         <v>2011</v>
       </c>
-      <c r="L1" s="1">
+      <c r="M1" s="1">
         <v>2010</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N1" s="1">
         <v>2009</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="1">
         <v>2008</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="1">
         <v>2007</v>
       </c>
-      <c r="P1" s="1">
+      <c r="Q1" s="1">
         <v>2006</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="R1" s="1">
         <v>2005</v>
       </c>
-      <c r="R1" s="1">
+      <c r="S1" s="1">
         <v>2004</v>
       </c>
-      <c r="S1" s="1">
+      <c r="T1" s="1">
         <v>2003</v>
       </c>
-      <c r="T1" s="1">
+      <c r="U1" s="1">
         <v>2002</v>
       </c>
-      <c r="U1" s="1">
+      <c r="V1" s="1">
         <v>2001</v>
       </c>
-      <c r="V1" s="1">
+      <c r="W1" s="1">
         <v>2000</v>
       </c>
-      <c r="W1" s="1">
+      <c r="X1" s="1">
         <v>1999</v>
       </c>
-      <c r="X1" s="1">
+      <c r="Y1" s="1">
         <v>1998</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Z1" s="1">
         <v>1997</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="AA1" s="1">
         <v>1996</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AB1" s="1">
         <v>1995</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AC1" s="1">
         <v>1994</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AD1" s="1">
         <v>1993</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AE1" s="1">
         <v>1992</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AF1" s="1">
         <v>1991</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AG1" s="1">
         <v>1990</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="AH1" s="1">
         <v>1989</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="AI1" s="1">
         <v>1988</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AJ1" s="1">
         <v>1987</v>
       </c>
-      <c r="AJ1" s="1">
+      <c r="AK1" s="1">
         <v>1986</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AL1" s="1">
         <v>1985</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AM1" s="1">
         <v>1984</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AN1" s="1">
         <v>1983</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AO1" s="1">
         <v>1982</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AP1" s="1">
         <v>1981</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AQ1" s="1">
         <v>1980</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3347,7 +3428,7 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>105000</v>
       </c>
       <c r="E2" s="2">
@@ -3357,22 +3438,22 @@
         <v>105000</v>
       </c>
       <c r="G2" s="2">
+        <v>105000</v>
+      </c>
+      <c r="H2" s="2">
         <v>107820</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>104100</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>105000</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>104140</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <v>103940</v>
-      </c>
-      <c r="L2" s="2">
-        <v>105000</v>
       </c>
       <c r="M2" s="2">
         <v>105000</v>
@@ -3384,58 +3465,61 @@
         <v>105000</v>
       </c>
       <c r="P2" s="2">
+        <v>105000</v>
+      </c>
+      <c r="Q2" s="2">
         <v>101160</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="R2" s="2">
         <v>101940</v>
       </c>
-      <c r="R2" s="2">
+      <c r="S2" s="2">
         <v>101900</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>105130</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>104940</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>106880</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>109460</v>
       </c>
-      <c r="W2" s="2">
+      <c r="X2" s="2">
         <v>108500</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <v>107160</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Z2" s="2">
         <v>97740</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AA2" s="2">
         <v>90880</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AB2" s="2">
         <v>74570</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AC2" s="2">
         <v>72870</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AD2" s="2">
         <v>54830</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AE2" s="2">
         <v>33929</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AF2" s="2">
         <v>26700</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AG2" s="2">
         <v>6110</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -3445,41 +3529,41 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>0</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
       </c>
       <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>14626</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>6715</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>19795</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>6693</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>10463</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>4000</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>8000</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>12000</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>16000</v>
-      </c>
-      <c r="O3" s="2">
-        <v>20000</v>
       </c>
       <c r="P3" s="2">
         <v>20000</v>
@@ -3490,8 +3574,11 @@
       <c r="R3" s="2">
         <v>20000</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="S3" s="2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -3501,11 +3588,11 @@
       <c r="C4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
+        <v>160000</v>
+      </c>
+      <c r="E4" s="2">
         <v>130000</v>
-      </c>
-      <c r="E4" s="2">
-        <v>100000</v>
       </c>
       <c r="F4" s="2">
         <v>100000</v>
@@ -3520,34 +3607,37 @@
         <v>100000</v>
       </c>
       <c r="J4" s="2">
+        <v>100000</v>
+      </c>
+      <c r="K4" s="2">
         <v>106722</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <v>63278</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>70000</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>60000</v>
-      </c>
-      <c r="N4" s="2">
-        <v>50000</v>
       </c>
       <c r="O4" s="2">
         <v>50000</v>
       </c>
       <c r="P4" s="2">
+        <v>50000</v>
+      </c>
+      <c r="Q4" s="2">
         <v>40000</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>30000</v>
       </c>
-      <c r="R4" s="2">
+      <c r="S4" s="2">
         <v>35000</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -3557,54 +3647,57 @@
       <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
         <v>105311</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>130796</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>153327</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>89168</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>71398</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <v>15182</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <v>0</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <f>33761+46546</f>
         <v>80307</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>30133</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>26085</v>
       </c>
-      <c r="O5" s="2">
+      <c r="P5" s="2">
         <v>25021</v>
       </c>
-      <c r="P5" s="2">
+      <c r="Q5" s="2">
         <v>20000</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>15000</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <v>14359</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
@@ -3614,41 +3707,44 @@
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
+        <v>68000</v>
+      </c>
+      <c r="E6" s="2">
         <v>63000</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>45000</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>41000</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>36000</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>31000</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>26000</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>21000</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <v>16000</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>6809</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>8000</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <v>4000</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -3658,11 +3754,12 @@
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="2">
+      <c r="D7" s="3"/>
+      <c r="K7" s="2">
         <v>448</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -3672,23 +3769,24 @@
       <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3"/>
+      <c r="E8" s="2">
         <v>87594</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>23555</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>56232</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>38313</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>18868</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -3698,50 +3796,53 @@
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
+        <v>44477</v>
+      </c>
+      <c r="E9" s="2">
         <v>95752</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>119379</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>125432</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>94477</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>43010</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>32750</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>73662</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>122216</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>148614</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>144325</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>94303</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>65310</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>102039</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="R9" s="2">
         <v>108666</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -3751,17 +3852,17 @@
       <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>56200</v>
       </c>
       <c r="E10" s="2">
         <v>56200</v>
       </c>
       <c r="F10" s="2">
+        <v>56200</v>
+      </c>
+      <c r="G10" s="2">
         <v>67700</v>
-      </c>
-      <c r="G10" s="2">
-        <v>56200</v>
       </c>
       <c r="H10" s="2">
         <v>56200</v>
@@ -3779,13 +3880,16 @@
         <v>56200</v>
       </c>
       <c r="M10" s="2">
+        <v>56200</v>
+      </c>
+      <c r="N10" s="2">
         <v>54429</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>7385</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -3795,47 +3899,50 @@
       <c r="C11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
+        <v>21511</v>
+      </c>
+      <c r="E11" s="2">
         <v>21546</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>23126</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>22070</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>23147</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>23923</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>24056</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>23939</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>23765</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>25307</v>
       </c>
-      <c r="M11" s="2">
+      <c r="N11" s="2">
         <v>25759</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>23197</v>
       </c>
-      <c r="O11" s="2">
+      <c r="P11" s="2">
         <v>23125</v>
       </c>
-      <c r="P11" s="2">
+      <c r="Q11" s="2">
         <v>687</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -3845,11 +3952,11 @@
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T12" s="2">
         <v>40590</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -3859,11 +3966,11 @@
       <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="S13" s="2">
+      <c r="T13" s="2">
         <v>3114</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>33</v>
       </c>
@@ -3873,11 +3980,11 @@
       <c r="C14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="S14" s="2">
+      <c r="T14" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -3887,25 +3994,25 @@
       <c r="C15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>151507</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <v>140188</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>80582</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <v>73125</v>
       </c>
-      <c r="P15" s="2">
+      <c r="Q15" s="2">
         <v>40842</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="R15" s="2">
         <v>30000</v>
       </c>
-      <c r="R15" s="2">
+      <c r="S15" s="2">
         <v>20000</v>
       </c>
     </row>

</xml_diff>